<commit_message>
updating results for ILAsimLIN and OLGsimLIM
</commit_message>
<xml_diff>
--- a/OLG/OLG Table.xlsx
+++ b/OLG/OLG Table.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/klp4/Dropbox/Papers/5 in progress/Policy Uncertainty/Python Code/OLG/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14160" yWindow="465" windowWidth="10185" windowHeight="15000" activeTab="1"/>
+    <workbookView xWindow="14160" yWindow="460" windowWidth="10180" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="GSSA" sheetId="5" r:id="rId3"/>
     <sheet name="VFI" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>LIN</t>
   </si>
@@ -45,9 +50,6 @@
     <t>OPFE</t>
   </si>
   <si>
-    <t>Euler errors</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -85,16 +87,82 @@
   </si>
   <si>
     <t>RMSEE</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>k3</t>
+  </si>
+  <si>
+    <t>k4</t>
+  </si>
+  <si>
+    <t>l1</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>l3</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>c3</t>
+  </si>
+  <si>
+    <t>c4</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>u2</t>
+  </si>
+  <si>
+    <t>u3</t>
+  </si>
+  <si>
+    <t>u4</t>
+  </si>
+  <si>
+    <t>Capital</t>
+  </si>
+  <si>
+    <t>Labor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -453,7 +521,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -463,13 +531,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -480,28 +548,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <f>AVERAGE(LIN!C3:C5)</f>
+        <v>2.7704266666666668E-2</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f>AVERAGE(LIN!D3:D5)</f>
+        <v>0.96596299999999991</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,61 +583,77 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f>AVERAGE(LIN!E3:E5)</f>
+        <v>3.6739466666666662</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f>AVERAGE(LIN!F3:F5)</f>
+        <v>11.054266666666665</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="B9" s="3">
+        <f>AVERAGE(LIN!H3:H5)</f>
+        <v>3.0801733333333338E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="3">
+        <f>AVERAGE(LIN!H6:H8)</f>
+        <v>5.1971433333333338E-4</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5">
-        <v>1.5061661383072E-2</v>
+        <v>3.5265878209124344E-4</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4">
-        <v>2027.14597075695</v>
+        <v>19.539120268242446</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -576,15 +666,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H8"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8">
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -592,10 +682,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -609,86 +699,432 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8">
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.5090999999999999E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.72617</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.10867</v>
+      </c>
+      <c r="F3" s="2">
+        <v>21.440999999999999</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>1.6258599999999999E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2.67237E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.81183899999999998</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2.6739099999999998</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8.0023499999999999</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>4.4515800000000002E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.12981E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.35987999999999998</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.23926</v>
+      </c>
+      <c r="F5" s="2">
+        <v>3.7194500000000001</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5">
+        <v>3.1630800000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9.2239700000000004E-4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.6582499999999997E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.9063499999999995E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.332872</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>3.9660200000000002E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2">
+        <v>7.7490100000000004E-4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.1776600000000002E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7.0959099999999997E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.29896099999999998</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7">
+        <v>6.2467800000000004E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.41628E-3</v>
+      </c>
+      <c r="D8" s="2">
+        <v>6.2954700000000002E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.15145700000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.64201600000000003</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8">
+        <v>5.3786299999999997E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.04691E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.32053199999999998</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.8524399999999999E-4</v>
+      </c>
+      <c r="D10" s="2">
+        <v>7.71508E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.60688E-4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5.7725699999999997E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="C11" s="2">
+        <v>6.2441099999999995E-4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2.5766799999999999E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.7695300000000001E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2.2172699999999999E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C12" s="2">
+        <v>5.9242699999999997E-3</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.17366699999999999</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.57717E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1.97623E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="C13" s="2">
+        <v>1.53666E-4</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6.8970300000000002E-3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5.1517499999999999E-4</v>
+      </c>
+      <c r="F13" s="2">
+        <v>6.4552800000000003E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.92126E-2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.792825</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5.4447200000000001E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6.8223699999999998E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2">
+        <v>3.1820300000000003E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.3233900000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <v>8.3886600000000006E-2</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.105112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.3931899999999999E-3</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.144763</v>
+      </c>
+      <c r="E16" s="2">
+        <v>9.0082200000000008E-3</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1.12876E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.5824200000000002E-3</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.110724</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6.7943400000000003E-3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>8.5134600000000005E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1.94287E-3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8.4202200000000005E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5.1201800000000002E-3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6.41568E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.5477100000000001E-3</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6.5890099999999993E-2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>4.3123800000000002E-3</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5.4035100000000003E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2">
+        <v>6.08879E-4</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2.6099600000000001E-2</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.6359600000000001E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2.04989E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.0100100000000001E-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.80340800000000001</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.11756999999999999</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.14733499999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4.30083E-5</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.48898E-3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.13331E-4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1.4200700000000001E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4.5838899999999999E-5</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.6198E-3</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1.15466E-4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.4468200000000001E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="2">
+        <v>8.75963E-5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3.2151599999999999E-3</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2.24193E-4</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2.80921E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.6426599999999998E-4</v>
+      </c>
+      <c r="D25" s="2">
+        <v>9.1855200000000008E-3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>7.3624200000000002E-4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>9.2252800000000004E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -704,9 +1140,9 @@
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -714,7 +1150,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -728,77 +1164,77 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -818,9 +1254,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -828,7 +1264,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -842,77 +1278,77 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>

</xml_diff>